<commit_message>
major update to readme converted readme from markup to reStructuredText
</commit_message>
<xml_diff>
--- a/thoipapy/setting/hydrophobicity_scales.xlsx
+++ b/thoipapy/setting/hydrophobicity_scales.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python_modules\thoipapy\thoipapy\setting\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="16635" windowHeight="10545"/>
+    <workbookView xWindow="3030" yWindow="120" windowWidth="16635" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Ile</t>
   </si>
@@ -187,12 +192,27 @@
   </si>
   <si>
     <t>Engelman(GES)</t>
+  </si>
+  <si>
+    <t>Pilpel Y, Ben-Tal N, &amp; Lancet D (1999) KPROT: A knowledge-based scale for the propensity of residue orientation in transmembrane segments. Application to membrane protein structure prediction11Edited by G. von Heijne. J. Mol. Biol. 294(4):921-935.</t>
+  </si>
+  <si>
+    <t>kPROT_Extracellular</t>
+  </si>
+  <si>
+    <t>kPROT_Central</t>
+  </si>
+  <si>
+    <t>kPROT_Intracellular</t>
+  </si>
+  <si>
+    <t>kPROT_Both termini</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -255,6 +275,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -302,7 +325,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -337,7 +360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -546,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,12 +582,12 @@
     <col min="12" max="12" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>21</v>
       </c>
@@ -577,8 +600,20 @@
       <c r="F2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -615,8 +650,20 @@
       <c r="L3" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -653,8 +700,20 @@
       <c r="L4" s="3">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>0.03</v>
+      </c>
+      <c r="N4">
+        <v>0.09</v>
+      </c>
+      <c r="O4">
+        <v>0.18</v>
+      </c>
+      <c r="P4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -691,8 +750,20 @@
       <c r="L5" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>0.53</v>
+      </c>
+      <c r="N5">
+        <v>0.12</v>
+      </c>
+      <c r="O5">
+        <v>0.61</v>
+      </c>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -729,8 +800,20 @@
       <c r="L6" s="3">
         <v>-9.1999999999999993</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>1.35</v>
+      </c>
+      <c r="N6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O6">
+        <v>1.23</v>
+      </c>
+      <c r="P6">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -767,8 +850,20 @@
       <c r="L7" s="3">
         <v>-8.1999999999999993</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>1.01</v>
+      </c>
+      <c r="N7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O7">
+        <v>1.33</v>
+      </c>
+      <c r="P7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -805,8 +900,20 @@
       <c r="L8" s="3">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0.41</v>
+      </c>
+      <c r="N8">
+        <v>0.16</v>
+      </c>
+      <c r="O8">
+        <v>0.12</v>
+      </c>
+      <c r="P8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -843,8 +950,20 @@
       <c r="L9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0.02</v>
+      </c>
+      <c r="N9">
+        <v>0.05</v>
+      </c>
+      <c r="O9">
+        <v>0.33</v>
+      </c>
+      <c r="P9">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -881,8 +1000,20 @@
       <c r="L10" s="3">
         <v>-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>0.21</v>
+      </c>
+      <c r="N10">
+        <v>0.69</v>
+      </c>
+      <c r="O10">
+        <v>0.21</v>
+      </c>
+      <c r="P10">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -919,8 +1050,20 @@
       <c r="L11" s="3">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>0.34</v>
+      </c>
+      <c r="N11">
+        <v>0.12</v>
+      </c>
+      <c r="O11">
+        <v>0.09</v>
+      </c>
+      <c r="P11">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -957,8 +1100,20 @@
       <c r="L12" s="3">
         <v>-8.8000000000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>0.85</v>
+      </c>
+      <c r="N12">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O12">
+        <v>0.66</v>
+      </c>
+      <c r="P12">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -995,8 +1150,20 @@
       <c r="L13" s="3">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>0.11</v>
+      </c>
+      <c r="N13">
+        <v>0.26</v>
+      </c>
+      <c r="O13">
+        <v>0.17</v>
+      </c>
+      <c r="P13">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1033,8 +1200,20 @@
       <c r="L14" s="3">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N14">
+        <v>0.39</v>
+      </c>
+      <c r="O14">
+        <v>0.32</v>
+      </c>
+      <c r="P14">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1071,8 +1250,20 @@
       <c r="L15" s="3">
         <v>-4.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>0.69</v>
+      </c>
+      <c r="N15">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="O15">
+        <v>0.75</v>
+      </c>
+      <c r="P15">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1109,8 +1300,20 @@
       <c r="L16" s="3">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>0.16</v>
+      </c>
+      <c r="N16">
+        <v>0.66</v>
+      </c>
+      <c r="O16">
+        <v>0.75</v>
+      </c>
+      <c r="P16">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1147,8 +1350,20 @@
       <c r="L17" s="3">
         <v>-4.0999999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>0.78</v>
+      </c>
+      <c r="N17">
+        <v>0.83</v>
+      </c>
+      <c r="O17">
+        <v>0.39</v>
+      </c>
+      <c r="P17">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1185,8 +1400,20 @@
       <c r="L18" s="3">
         <v>-12.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>0.53</v>
+      </c>
+      <c r="N18">
+        <v>0.84</v>
+      </c>
+      <c r="O18">
+        <v>0.44</v>
+      </c>
+      <c r="P18">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1223,8 +1450,20 @@
       <c r="L19" s="3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>0.11</v>
+      </c>
+      <c r="N19">
+        <v>0.22</v>
+      </c>
+      <c r="O19">
+        <v>0.41</v>
+      </c>
+      <c r="P19">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1261,8 +1500,20 @@
       <c r="L20" s="3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>0.03</v>
+      </c>
+      <c r="N20">
+        <v>0.03</v>
+      </c>
+      <c r="O20">
+        <v>0.43</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1299,8 +1550,20 @@
       <c r="L21" s="3">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>0.27</v>
+      </c>
+      <c r="N21">
+        <v>0.31</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1337,8 +1600,20 @@
       <c r="L22" s="3">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>0.25</v>
+      </c>
+      <c r="N22">
+        <v>0.65</v>
+      </c>
+      <c r="O22">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="P22">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1374,6 +1649,18 @@
       </c>
       <c r="L23" s="3">
         <v>-0.7</v>
+      </c>
+      <c r="M23">
+        <v>0.18</v>
+      </c>
+      <c r="N23">
+        <v>0.7</v>
+      </c>
+      <c r="O23">
+        <v>0.26</v>
+      </c>
+      <c r="P23">
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>